<commit_message>
content by Mario added
</commit_message>
<xml_diff>
--- a/besitzkarten.xlsx
+++ b/besitzkarten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\DKT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94693B15-90B1-4CB1-A693-4530FD6EF6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A6608A-D2B0-4A23-8E37-D88727BF8F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4147E4F9-C290-4137-B84E-9B6C097A9EB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{4147E4F9-C290-4137-B84E-9B6C097A9EB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -78,6 +78,114 @@
   </si>
   <si>
     <t>#7F0000</t>
+  </si>
+  <si>
+    <t>Käsemacher</t>
+  </si>
+  <si>
+    <t>Schlosserbäck</t>
+  </si>
+  <si>
+    <t>Ypsilon</t>
+  </si>
+  <si>
+    <t>Bauhof</t>
+  </si>
+  <si>
+    <t>Drachenschanze</t>
+  </si>
+  <si>
+    <t>Gebharter</t>
+  </si>
+  <si>
+    <t>GH. Stille Post</t>
+  </si>
+  <si>
+    <t>Lagerhaus</t>
+  </si>
+  <si>
+    <t>Disco Löffler</t>
+  </si>
+  <si>
+    <t>Hanfhalle</t>
+  </si>
+  <si>
+    <t>Volksschule</t>
+  </si>
+  <si>
+    <t>Fußballplatz</t>
+  </si>
+  <si>
+    <t>Bäck Garage</t>
+  </si>
+  <si>
+    <t>Leop. Teich</t>
+  </si>
+  <si>
+    <t>Weinstabl</t>
+  </si>
+  <si>
+    <t>Pflegeheim</t>
+  </si>
+  <si>
+    <t>Flugplatz Wald</t>
+  </si>
+  <si>
+    <t>Dienststelle</t>
+  </si>
+  <si>
+    <t>Wirtshaus</t>
+  </si>
+  <si>
+    <t>Schrammelhof</t>
+  </si>
+  <si>
+    <t>Jamaikabar</t>
+  </si>
+  <si>
+    <t>Tschick-Toni</t>
+  </si>
+  <si>
+    <t>#0094FF</t>
+  </si>
+  <si>
+    <t>#FF006E</t>
+  </si>
+  <si>
+    <t>#FF6A00</t>
+  </si>
+  <si>
+    <t>#FF0000</t>
+  </si>
+  <si>
+    <t>#FFCC00</t>
+  </si>
+  <si>
+    <t>#007F0E</t>
+  </si>
+  <si>
+    <t>#00137F</t>
+  </si>
+  <si>
+    <t>KH Gmünd</t>
+  </si>
+  <si>
+    <t>KH Waidhofen</t>
+  </si>
+  <si>
+    <t>KH Zwettl</t>
+  </si>
+  <si>
+    <t>KH Horn</t>
+  </si>
+  <si>
+    <t>#404040</t>
+  </si>
+  <si>
+    <t>IstBahnhof</t>
+  </si>
+  <si>
+    <t>IstWerk</t>
   </si>
 </sst>
 </file>
@@ -449,15 +557,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88B7BA2-66B4-4DC5-B23B-8AA88540F6D8}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D27" sqref="D27:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +599,14 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -527,7 +641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -560,6 +674,886 @@
       </c>
       <c r="K3">
         <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <v>290</v>
+      </c>
+      <c r="J4">
+        <v>90</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="I5">
+        <v>290</v>
+      </c>
+      <c r="J5">
+        <v>90</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="G6">
+        <v>120</v>
+      </c>
+      <c r="H6">
+        <v>240</v>
+      </c>
+      <c r="I6">
+        <v>330</v>
+      </c>
+      <c r="J6">
+        <v>110</v>
+      </c>
+      <c r="K6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>140</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="G7">
+        <v>140</v>
+      </c>
+      <c r="H7">
+        <v>280</v>
+      </c>
+      <c r="I7">
+        <v>370</v>
+      </c>
+      <c r="J7">
+        <v>120</v>
+      </c>
+      <c r="K7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>140</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>80</v>
+      </c>
+      <c r="G8">
+        <v>140</v>
+      </c>
+      <c r="H8">
+        <v>280</v>
+      </c>
+      <c r="I8">
+        <v>370</v>
+      </c>
+      <c r="J8">
+        <v>120</v>
+      </c>
+      <c r="K8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>140</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>80</v>
+      </c>
+      <c r="G9">
+        <v>140</v>
+      </c>
+      <c r="H9">
+        <v>280</v>
+      </c>
+      <c r="I9">
+        <v>370</v>
+      </c>
+      <c r="J9">
+        <v>120</v>
+      </c>
+      <c r="K9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>180</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>180</v>
+      </c>
+      <c r="H10">
+        <v>360</v>
+      </c>
+      <c r="I10">
+        <v>450</v>
+      </c>
+      <c r="J10">
+        <v>140</v>
+      </c>
+      <c r="K10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>180</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>180</v>
+      </c>
+      <c r="H11">
+        <v>360</v>
+      </c>
+      <c r="I11">
+        <v>450</v>
+      </c>
+      <c r="J11">
+        <v>140</v>
+      </c>
+      <c r="K11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>60</v>
+      </c>
+      <c r="F12">
+        <v>120</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12">
+        <v>400</v>
+      </c>
+      <c r="I12">
+        <v>490</v>
+      </c>
+      <c r="J12">
+        <v>180</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>220</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>120</v>
+      </c>
+      <c r="G13">
+        <v>220</v>
+      </c>
+      <c r="H13">
+        <v>440</v>
+      </c>
+      <c r="I13">
+        <v>530</v>
+      </c>
+      <c r="J13">
+        <v>200</v>
+      </c>
+      <c r="K13">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>220</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>60</v>
+      </c>
+      <c r="F14">
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <v>220</v>
+      </c>
+      <c r="H14">
+        <v>440</v>
+      </c>
+      <c r="I14">
+        <v>530</v>
+      </c>
+      <c r="J14">
+        <v>200</v>
+      </c>
+      <c r="K14">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>240</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>70</v>
+      </c>
+      <c r="F15">
+        <v>140</v>
+      </c>
+      <c r="G15">
+        <v>240</v>
+      </c>
+      <c r="H15">
+        <v>480</v>
+      </c>
+      <c r="I15">
+        <v>570</v>
+      </c>
+      <c r="J15">
+        <v>220</v>
+      </c>
+      <c r="K15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>260</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>70</v>
+      </c>
+      <c r="F16">
+        <v>140</v>
+      </c>
+      <c r="G16">
+        <v>260</v>
+      </c>
+      <c r="H16">
+        <v>520</v>
+      </c>
+      <c r="I16">
+        <v>610</v>
+      </c>
+      <c r="J16">
+        <v>230</v>
+      </c>
+      <c r="K16">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>260</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>70</v>
+      </c>
+      <c r="F17">
+        <v>140</v>
+      </c>
+      <c r="G17">
+        <v>260</v>
+      </c>
+      <c r="H17">
+        <v>520</v>
+      </c>
+      <c r="I17">
+        <v>610</v>
+      </c>
+      <c r="J17">
+        <v>230</v>
+      </c>
+      <c r="K17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>280</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <v>160</v>
+      </c>
+      <c r="G18">
+        <v>280</v>
+      </c>
+      <c r="H18">
+        <v>560</v>
+      </c>
+      <c r="I18">
+        <v>650</v>
+      </c>
+      <c r="J18">
+        <v>240</v>
+      </c>
+      <c r="K18">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>300</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>200</v>
+      </c>
+      <c r="G19">
+        <v>300</v>
+      </c>
+      <c r="H19">
+        <v>600</v>
+      </c>
+      <c r="I19">
+        <v>690</v>
+      </c>
+      <c r="J19">
+        <v>260</v>
+      </c>
+      <c r="K19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>300</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>200</v>
+      </c>
+      <c r="G20">
+        <v>300</v>
+      </c>
+      <c r="H20">
+        <v>600</v>
+      </c>
+      <c r="I20">
+        <v>690</v>
+      </c>
+      <c r="J20">
+        <v>260</v>
+      </c>
+      <c r="K20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>320</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>120</v>
+      </c>
+      <c r="F21">
+        <v>240</v>
+      </c>
+      <c r="G21">
+        <v>320</v>
+      </c>
+      <c r="H21">
+        <v>640</v>
+      </c>
+      <c r="I21">
+        <v>730</v>
+      </c>
+      <c r="J21">
+        <v>280</v>
+      </c>
+      <c r="K21">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22">
+        <v>350</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>130</v>
+      </c>
+      <c r="F22">
+        <v>260</v>
+      </c>
+      <c r="G22">
+        <v>350</v>
+      </c>
+      <c r="H22">
+        <v>700</v>
+      </c>
+      <c r="I22">
+        <v>790</v>
+      </c>
+      <c r="J22">
+        <v>300</v>
+      </c>
+      <c r="K22">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23">
+        <v>400</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>150</v>
+      </c>
+      <c r="F23">
+        <v>300</v>
+      </c>
+      <c r="G23">
+        <v>400</v>
+      </c>
+      <c r="H23">
+        <v>800</v>
+      </c>
+      <c r="I23">
+        <v>890</v>
+      </c>
+      <c r="J23">
+        <v>350</v>
+      </c>
+      <c r="K23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>150</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>150</v>
+      </c>
+      <c r="G25">
+        <v>200</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26">
+        <v>200</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>150</v>
+      </c>
+      <c r="G26">
+        <v>200</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>200</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>150</v>
+      </c>
+      <c r="G27">
+        <v>200</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>150</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>80</v>
+      </c>
+      <c r="G28">
+        <v>150</v>
+      </c>
+      <c r="H28">
+        <v>300</v>
+      </c>
+      <c r="I28">
+        <v>390</v>
+      </c>
+      <c r="J28">
+        <v>130</v>
+      </c>
+      <c r="K28">
+        <v>75</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>150</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <v>80</v>
+      </c>
+      <c r="G29">
+        <v>150</v>
+      </c>
+      <c r="H29">
+        <v>300</v>
+      </c>
+      <c r="I29">
+        <v>390</v>
+      </c>
+      <c r="J29">
+        <v>130</v>
+      </c>
+      <c r="K29">
+        <v>75</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>